<commit_message>
modify parameter for clear result
</commit_message>
<xml_diff>
--- a/Delay Model/main.xlsx
+++ b/Delay Model/main.xlsx
@@ -383,10 +383,10 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1956.011502714073</v>
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>80.076374499316472</v>
+        <v>0</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -395,10 +395,10 @@
         <v>0</v>
       </c>
       <c r="F1">
-        <v>1.5753771016858997</v>
+        <v>0</v>
       </c>
       <c r="G1">
-        <v>42.273732660301839</v>
+        <v>0</v>
       </c>
       <c r="H1">
         <v>0</v>
@@ -407,7 +407,7 @@
         <v>0</v>
       </c>
       <c r="J1">
-        <v>80.076374499316472</v>
+        <v>76.570724343257581</v>
       </c>
       <c r="K1">
         <v>0</v>
@@ -416,10 +416,10 @@
         <v>0</v>
       </c>
       <c r="M1">
-        <v>6.600239501881597E-3</v>
+        <v>6.3064123963058666E-3</v>
       </c>
       <c r="N1">
-        <v>50.635732660301819</v>
+        <v>49.471903250931668</v>
       </c>
       <c r="O1">
         <v>0</v>
@@ -428,7 +428,7 @@
         <v>0</v>
       </c>
       <c r="Q1">
-        <v>80.076374499316472</v>
+        <v>76.570724343257581</v>
       </c>
       <c r="R1">
         <v>0</v>
@@ -437,10 +437,10 @@
         <v>0</v>
       </c>
       <c r="T1">
-        <v>6.1838134274653477E-3</v>
+        <v>1.0059653637984452E-2</v>
       </c>
       <c r="U1">
-        <v>48.49873266030184</v>
+        <v>49.471903250931668</v>
       </c>
       <c r="V1">
         <v>0</v>
@@ -449,7 +449,7 @@
         <v>0</v>
       </c>
       <c r="X1">
-        <v>80.076374499316472</v>
+        <v>76.570724343257581</v>
       </c>
       <c r="Y1">
         <v>0</v>
@@ -458,10 +458,10 @@
         <v>0</v>
       </c>
       <c r="AA1">
-        <v>2.9876295287046703E-2</v>
+        <v>3.1286871079647789E-2</v>
       </c>
       <c r="AB1">
-        <v>50.242732660301833</v>
+        <v>49.471903250931668</v>
       </c>
       <c r="AC1">
         <v>0</v>
@@ -475,10 +475,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>18520.394256300813</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>203.04871879933182</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -487,10 +487,10 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>7.3460074012339183</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>145.48924656315407</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -499,7 +499,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>2048.0871299300793</v>
+        <v>2032.5822270573306</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -508,10 +508,10 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>1.0001905775067342E-2</v>
+        <v>1.6018759663991754E-2</v>
       </c>
       <c r="N2">
-        <v>2004.8797339034493</v>
+        <v>2007.005405965006</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -520,7 +520,7 @@
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>214.33229375914215</v>
+        <v>209.81118823065617</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -529,10 +529,10 @@
         <v>0</v>
       </c>
       <c r="T2">
-        <v>1.231642692774837E-2</v>
+        <v>1.8372819877415927E-2</v>
       </c>
       <c r="U2">
-        <v>122.63849006092858</v>
+        <v>121.8368094235322</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -541,7 +541,7 @@
         <v>0</v>
       </c>
       <c r="X2">
-        <v>214.33229375914215</v>
+        <v>209.81118823065617</v>
       </c>
       <c r="Y2">
         <v>0</v>
@@ -550,10 +550,10 @@
         <v>0</v>
       </c>
       <c r="AA2">
-        <v>5.4457095883241408E-2</v>
+        <v>6.0741068167621828E-2</v>
       </c>
       <c r="AB2">
-        <v>115.53949006092857</v>
+        <v>121.8368094235322</v>
       </c>
       <c r="AC2">
         <v>0</v>
@@ -567,10 +567,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>20476.405759014888</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>331.66716010433004</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -579,10 +579,10 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>24.229973006260614</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>264.53038310184348</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -591,49 +591,49 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>19325.846952744021</v>
+        <v>20373.599423022504</v>
       </c>
       <c r="K3">
-        <v>17051.570481633407</v>
+        <v>18182.944399996137</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M3">
-        <v>1.5968119512007804E-2</v>
+        <v>1.4667934150029526E-2</v>
       </c>
       <c r="N3">
-        <v>19162.709745073473</v>
+        <v>20300.953409663798</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>17456.394622441705</v>
+        <v>18510.346990778009</v>
       </c>
       <c r="R3">
-        <v>17051.570481633407</v>
+        <v>18182.944399996137</v>
       </c>
       <c r="S3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T3">
-        <v>1.7616757167278695E-2</v>
+        <v>1.71738875671715E-2</v>
       </c>
       <c r="U3">
-        <v>17275.220501230917</v>
+        <v>18419.20281312232</v>
       </c>
       <c r="V3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W3">
         <v>0</v>
       </c>
       <c r="X3">
-        <v>385.1923098289945</v>
+        <v>892.29741555146859</v>
       </c>
       <c r="Y3">
         <v>0</v>
@@ -642,10 +642,10 @@
         <v>0</v>
       </c>
       <c r="AA3">
-        <v>3.3157926175393884E-2</v>
+        <v>2.3998557299008884E-2</v>
       </c>
       <c r="AB3">
-        <v>275.64356363363493</v>
+        <v>418.32270975413138</v>
       </c>
       <c r="AC3">
         <v>0</v>
@@ -659,10 +659,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>37040.788512601626</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>456.53145833501236</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -671,10 +671,10 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>44.625317510659542</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>378.10498877606119</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -683,49 +683,49 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>19738.238506513586</v>
+        <v>20915.296883265106</v>
       </c>
       <c r="K4">
-        <v>17254.56536831952</v>
+        <v>18536.466660293354</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M4">
-        <v>2.1353498519468772E-2</v>
+        <v>3.5543863002570238E-2</v>
       </c>
       <c r="N4">
-        <v>19513.05926327674</v>
+        <v>20802.088707995001</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>18041.022673223721</v>
+        <v>19244.538922948941</v>
       </c>
       <c r="R4">
-        <v>17254.56536831952</v>
+        <v>18536.466660293354</v>
       </c>
       <c r="S4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T4">
-        <v>2.6605757716255691E-2</v>
+        <v>2.3055624770311308E-2</v>
       </c>
       <c r="U4">
-        <v>17624.09101943421</v>
+        <v>18921.309111453545</v>
       </c>
       <c r="V4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W4">
         <v>0</v>
       </c>
       <c r="X4">
-        <v>582.54462569278871</v>
+        <v>532.63102317939195</v>
       </c>
       <c r="Y4">
         <v>0</v>
@@ -734,10 +734,10 @@
         <v>0</v>
       </c>
       <c r="AA4">
-        <v>6.0868464542628203E-2</v>
+        <v>4.1771768799201733E-2</v>
       </c>
       <c r="AB4">
-        <v>384.0048961435337</v>
+        <v>390.33571677624673</v>
       </c>
       <c r="AC4">
         <v>0</v>
@@ -751,10 +751,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>38996.800015315697</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>549.49107783267357</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -763,10 +763,10 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>56.37677457525394</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>360.2501889686975</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -775,49 +775,49 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>20061.25899758884</v>
+        <v>21408.914923198958</v>
       </c>
       <c r="K5">
-        <v>17484.626239897112</v>
+        <v>18937.125221963535</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M5">
-        <v>2.8412546257711987E-2</v>
+        <v>4.4440993188130259E-2</v>
       </c>
       <c r="N5">
-        <v>19717.931335046978</v>
+        <v>21156.25512321986</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>18364.043164298972</v>
+        <v>19853.217784146193</v>
       </c>
       <c r="R5">
-        <v>17484.626239897112</v>
+        <v>18937.125221963535</v>
       </c>
       <c r="S5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T5">
-        <v>3.3954653931158853E-2</v>
+        <v>2.8037664963414786E-2</v>
       </c>
       <c r="U5">
-        <v>17837.085091204448</v>
+        <v>19280.140526678369</v>
       </c>
       <c r="V5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W5">
         <v>0</v>
       </c>
       <c r="X5">
-        <v>718.24966883527088</v>
+        <v>630.70438594655207</v>
       </c>
       <c r="Y5">
         <v>0</v>
@@ -826,10 +826,10 @@
         <v>0</v>
       </c>
       <c r="AA5">
-        <v>4.1776865028458628E-2</v>
+        <v>5.2773786077480324E-2</v>
       </c>
       <c r="AB5">
-        <v>421.06327518876998</v>
+        <v>466.14830888783263</v>
       </c>
       <c r="AC5">
         <v>0</v>
@@ -843,10 +843,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>41502.117662363824</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>635.97418298874175</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -855,10 +855,10 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>103.92129632526745</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>416.35348886192503</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -867,49 +867,49 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>20403.807064862245</v>
+        <v>21945.177342471412</v>
       </c>
       <c r="K6">
-        <v>17747.552950271507</v>
+        <v>19395.020721015175</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M6">
-        <v>3.2558602583320773E-2</v>
+        <v>4.3475020679093465E-2</v>
       </c>
       <c r="N6">
-        <v>20045.585133322882</v>
+        <v>21676.381264704567</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>18873.579566026609</v>
+        <v>20437.49430504446</v>
       </c>
       <c r="R6">
-        <v>17747.552950271507</v>
+        <v>19395.020721015175</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T6">
-        <v>3.4195293588915786E-2</v>
+        <v>5.1096418619945003E-2</v>
       </c>
       <c r="U6">
-        <v>18158.454889480425</v>
+        <v>19794.551668163065</v>
       </c>
       <c r="V6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W6">
         <v>0</v>
       </c>
       <c r="X6">
-        <v>720.66054779175806</v>
+        <v>871.70748500309378</v>
       </c>
       <c r="Y6">
         <v>0</v>
@@ -918,10 +918,10 @@
         <v>0</v>
       </c>
       <c r="AA6">
-        <v>7.2433674760995895E-2</v>
+        <v>6.1822525022556425E-2</v>
       </c>
       <c r="AB6">
-        <v>414.2505462109537</v>
+        <v>730.25254414923518</v>
       </c>
       <c r="AC6">
         <v>0</v>
@@ -932,7 +932,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -959,49 +959,49 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>55328.337110708431</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>52685.207835165646</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>3.6970350674189648E-2</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>55045.102794036102</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P7">
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>53833.42940173544</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>52685.207835165653</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <v>3.9443308563932244E-2</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>53160.90119749459</v>
       </c>
       <c r="V7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W7">
         <v>0</v>
       </c>
       <c r="X7">
-        <v>0</v>
+        <v>1014.1532551878734</v>
       </c>
       <c r="Y7">
         <v>0</v>
@@ -1010,10 +1010,10 @@
         <v>0</v>
       </c>
       <c r="AA7">
-        <v>0</v>
+        <v>0.32835356869384358</v>
       </c>
       <c r="AB7">
-        <v>0</v>
+        <v>782.9718564620332</v>
       </c>
       <c r="AC7">
         <v>0</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1051,49 +1051,49 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>60567.736133916282</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>57781.636584276021</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>4.5575925552987971E-2</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>60226.4349094055</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>58994.062532449818</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>57781.636584276021</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>4.7037399861418784E-2</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>58345.031312864012</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W8">
         <v>0</v>
       </c>
       <c r="X8">
-        <v>0</v>
+        <v>1095.7786130443003</v>
       </c>
       <c r="Y8">
         <v>0</v>
@@ -1102,10 +1102,10 @@
         <v>0</v>
       </c>
       <c r="AA8">
-        <v>0</v>
+        <v>0.23251265492253448</v>
       </c>
       <c r="AB8">
-        <v>0</v>
+        <v>814.33781538367464</v>
       </c>
       <c r="AC8">
         <v>0</v>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1143,49 +1143,49 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>62483.26710327663</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>59618.170391417334</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>5.7682724110742094E-2</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>62118.431921620882</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>60943.880277231852</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>59618.170391417334</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>5.0879387694033613E-2</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>60240.592325079422</v>
       </c>
       <c r="V9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W9">
         <v>0</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>1227.4930050061523</v>
       </c>
       <c r="Y9">
         <v>0</v>
@@ -1194,10 +1194,10 @@
         <v>0</v>
       </c>
       <c r="AA9">
-        <v>0</v>
+        <v>1.0649252423749043</v>
       </c>
       <c r="AB9">
-        <v>0</v>
+        <v>874.93968417242274</v>
       </c>
       <c r="AC9">
         <v>0</v>
@@ -1208,7 +1208,7 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1235,49 +1235,49 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>71594.86295082829</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>66427.181145974944</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>5.2305875365653023E-2</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>71227.895769172654</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P10">
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>63263.301030696006</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>61822.010959986859</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>6.6884209592141142E-2</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>62547.437903997357</v>
       </c>
       <c r="V10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W10">
         <v>0</v>
       </c>
       <c r="X10">
-        <v>0</v>
+        <v>2826.1500983053807</v>
       </c>
       <c r="Y10">
         <v>0</v>
@@ -1286,10 +1286,10 @@
         <v>0</v>
       </c>
       <c r="AA10">
-        <v>0</v>
+        <v>1.9646083146453492</v>
       </c>
       <c r="AB10">
-        <v>0</v>
+        <v>1315.36879153985</v>
       </c>
       <c r="AC10">
         <v>0</v>
@@ -1300,7 +1300,7 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1327,49 +1327,49 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>82219.572299392763</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>74749.305401545382</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>5.4344202515169408E-2</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>81858.440117736987</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P11">
         <v>0</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>66474.616538476053</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>64515.593877127409</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T11">
-        <v>0</v>
+        <v>6.3872514384343285E-2</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>65349.934634289442</v>
       </c>
       <c r="V11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W11">
         <v>0</v>
       </c>
       <c r="X11">
-        <v>0</v>
+        <v>1592.3628330484526</v>
       </c>
       <c r="Y11">
         <v>0</v>
@@ -1378,10 +1378,10 @@
         <v>0</v>
       </c>
       <c r="AA11">
-        <v>0</v>
+        <v>7.4793399642965639</v>
       </c>
       <c r="AB11">
-        <v>0</v>
+        <v>1345.2175270453586</v>
       </c>
       <c r="AC11">
         <v>0</v>
@@ -1392,7 +1392,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1419,49 +1419,49 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>88821.7763890848</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>79395.497988523333</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>5.8377905739742657E-2</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>88445.919207429004</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P12">
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>88735.309131999209</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>86672.454876414064</v>
       </c>
       <c r="S12">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T12">
-        <v>0</v>
+        <v>6.9726376055714648E-2</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>87471.561876539388</v>
       </c>
       <c r="V12">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="W12">
         <v>0</v>
       </c>
       <c r="X12">
-        <v>0</v>
+        <v>1870.3338046630006</v>
       </c>
       <c r="Y12">
         <v>0</v>
@@ -1470,10 +1470,10 @@
         <v>0</v>
       </c>
       <c r="AA12">
-        <v>0</v>
+        <v>2.3509321805378725</v>
       </c>
       <c r="AB12">
-        <v>0</v>
+        <v>1458.9098576314186</v>
       </c>
       <c r="AC12">
         <v>0</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1511,64 +1511,64 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>94919.778452457758</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>85369.174171780687</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>6.6828458528604279E-2</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>94536.824523701041</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P13">
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>0</v>
+        <v>94142.852696075628</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>91896.183724335715</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T13">
-        <v>0</v>
+        <v>7.4912647185652173E-2</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>92808.291857475488</v>
       </c>
       <c r="V13">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="W13">
         <v>0</v>
       </c>
       <c r="X13">
-        <v>0</v>
+        <v>94142.852696075628</v>
       </c>
       <c r="Y13">
-        <v>0</v>
+        <v>91896.183724335715</v>
       </c>
       <c r="Z13">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA13">
-        <v>0</v>
+        <v>9.3393843148364954</v>
       </c>
       <c r="AB13">
-        <v>0</v>
+        <v>92808.291857475488</v>
       </c>
       <c r="AC13">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AD13">
         <v>0</v>
@@ -1576,7 +1576,7 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1603,64 +1603,64 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>104840.6915328483</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>93334.075749457159</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>6.8222235117026034E-2</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>104462.76260409155</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P14">
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>101224.33909343324</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>98861.155521564564</v>
       </c>
       <c r="S14">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <v>9.8176769555823315E-2</v>
       </c>
       <c r="U14">
-        <v>0</v>
+        <v>99858.264475064701</v>
       </c>
       <c r="V14">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="W14">
         <v>0</v>
       </c>
       <c r="X14">
-        <v>0</v>
+        <v>101224.33909343324</v>
       </c>
       <c r="Y14">
-        <v>0</v>
+        <v>98861.155521564564</v>
       </c>
       <c r="Z14">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA14">
-        <v>0</v>
+        <v>5.5232811890222742</v>
       </c>
       <c r="AB14">
-        <v>0</v>
+        <v>99858.264475064701</v>
       </c>
       <c r="AC14">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AD14">
         <v>0</v>
@@ -1668,7 +1668,7 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1695,64 +1695,64 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>147839.69232343382</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>136243.1371536135</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>7.4846371686651716E-2</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>147427.52406154003</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="P15">
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>142927.92483813508</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>140370.31523309427</v>
       </c>
       <c r="S15">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T15">
-        <v>0</v>
+        <v>8.7120138990814722E-2</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>141431.0912398865</v>
       </c>
       <c r="V15">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W15">
         <v>0</v>
       </c>
       <c r="X15">
-        <v>0</v>
+        <v>142927.92483813508</v>
       </c>
       <c r="Y15">
-        <v>0</v>
+        <v>140370.31523309427</v>
       </c>
       <c r="Z15">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA15">
-        <v>0</v>
+        <v>3.3074847509463456</v>
       </c>
       <c r="AB15">
-        <v>0</v>
+        <v>141431.0912398865</v>
       </c>
       <c r="AC15">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD15">
         <v>0</v>
@@ -1760,7 +1760,7 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1787,64 +1787,64 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>195258.01963256596</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>183498.59438313707</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>7.6387774815765488E-2</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>194738.77103953919</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P16">
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>187867.03657092812</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>185191.87757073811</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="T16">
-        <v>0</v>
+        <v>9.1602410721498412E-2</v>
       </c>
       <c r="U16">
-        <v>0</v>
+        <v>186309.6203260062</v>
       </c>
       <c r="V16">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="W16">
         <v>0</v>
       </c>
       <c r="X16">
-        <v>0</v>
+        <v>187867.03657092812</v>
       </c>
       <c r="Y16">
-        <v>0</v>
+        <v>185191.87757073811</v>
       </c>
       <c r="Z16">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AA16">
-        <v>0</v>
+        <v>1.5924986944011141</v>
       </c>
       <c r="AB16">
-        <v>0</v>
+        <v>186309.6203260062</v>
       </c>
       <c r="AC16">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AD16">
         <v>0</v>

</xml_diff>

<commit_message>
modify mainly on figure
</commit_message>
<xml_diff>
--- a/Delay Model/main.xlsx
+++ b/Delay Model/main.xlsx
@@ -383,10 +383,10 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>2738.4161037997023</v>
       </c>
       <c r="C1">
-        <v>0</v>
+        <v>87.154893034625118</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -395,10 +395,10 @@
         <v>0</v>
       </c>
       <c r="F1">
-        <v>0</v>
+        <v>0.74198600000000003</v>
       </c>
       <c r="G1">
-        <v>0</v>
+        <v>49.074665823675659</v>
       </c>
       <c r="H1">
         <v>0</v>
@@ -407,7 +407,7 @@
         <v>0</v>
       </c>
       <c r="J1">
-        <v>76.570724343257581</v>
+        <v>87.154893034625118</v>
       </c>
       <c r="K1">
         <v>0</v>
@@ -416,10 +416,10 @@
         <v>0</v>
       </c>
       <c r="M1">
-        <v>6.3064123963058666E-3</v>
+        <v>1.8541999999999999E-2</v>
       </c>
       <c r="N1">
-        <v>49.471903250931668</v>
+        <v>49.074665823675659</v>
       </c>
       <c r="O1">
         <v>0</v>
@@ -428,7 +428,7 @@
         <v>0</v>
       </c>
       <c r="Q1">
-        <v>76.570724343257581</v>
+        <v>87.154893034625118</v>
       </c>
       <c r="R1">
         <v>0</v>
@@ -437,10 +437,10 @@
         <v>0</v>
       </c>
       <c r="T1">
-        <v>1.0059653637984452E-2</v>
+        <v>1.7655000000000001E-2</v>
       </c>
       <c r="U1">
-        <v>49.471903250931668</v>
+        <v>49.074665823675659</v>
       </c>
       <c r="V1">
         <v>0</v>
@@ -449,7 +449,7 @@
         <v>0</v>
       </c>
       <c r="X1">
-        <v>76.570724343257581</v>
+        <v>87.154893034625118</v>
       </c>
       <c r="Y1">
         <v>0</v>
@@ -458,10 +458,10 @@
         <v>0</v>
       </c>
       <c r="AA1">
-        <v>3.1286871079647789E-2</v>
+        <v>5.6292000000000002E-2</v>
       </c>
       <c r="AB1">
-        <v>49.471903250931668</v>
+        <v>49.074665823675659</v>
       </c>
       <c r="AC1">
         <v>0</v>
@@ -475,10 +475,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>5476.8322075994047</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>158.26022119324031</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -487,10 +487,10 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1.8629800000000001</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>115.07382675119779</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -499,7 +499,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>2032.5822270573306</v>
+        <v>218.79218706988149</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -508,10 +508,10 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>1.6018759663991754E-2</v>
+        <v>2.6294000000000001E-2</v>
       </c>
       <c r="N2">
-        <v>2007.005405965006</v>
+        <v>94.532728427710666</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -520,7 +520,7 @@
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>209.81118823065617</v>
+        <v>195.69652910214413</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -529,10 +529,10 @@
         <v>0</v>
       </c>
       <c r="T2">
-        <v>1.8372819877415927E-2</v>
+        <v>2.3345000000000001E-2</v>
       </c>
       <c r="U2">
-        <v>121.8368094235322</v>
+        <v>94.532728427710666</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -541,7 +541,7 @@
         <v>0</v>
       </c>
       <c r="X2">
-        <v>209.81118823065617</v>
+        <v>195.69652910214413</v>
       </c>
       <c r="Y2">
         <v>0</v>
@@ -550,10 +550,10 @@
         <v>0</v>
       </c>
       <c r="AA2">
-        <v>6.0741068167621828E-2</v>
+        <v>9.3473000000000001E-2</v>
       </c>
       <c r="AB2">
-        <v>121.8368094235322</v>
+        <v>94.532728427710666</v>
       </c>
       <c r="AC2">
         <v>0</v>
@@ -567,10 +567,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>7229.6428614689576</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>289.95576606745817</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -579,10 +579,10 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>14.976967</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>232.7148193107144</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -591,49 +591,49 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>20373.599423022504</v>
+        <v>1461.4347887941162</v>
       </c>
       <c r="K3">
-        <v>18182.944399996137</v>
+        <v>460.23800063860551</v>
       </c>
       <c r="L3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>1.4667934150029526E-2</v>
+        <v>2.2422999999999998E-2</v>
       </c>
       <c r="N3">
-        <v>20300.953409663798</v>
+        <v>1342.9633301519443</v>
       </c>
       <c r="O3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>18510.346990778009</v>
+        <v>329.51769160123007</v>
       </c>
       <c r="R3">
-        <v>18182.944399996137</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>1.71738875671715E-2</v>
+        <v>2.4669E-2</v>
       </c>
       <c r="U3">
-        <v>18419.20281312232</v>
+        <v>215.45084598552162</v>
       </c>
       <c r="V3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W3">
         <v>0</v>
       </c>
       <c r="X3">
-        <v>892.29741555146859</v>
+        <v>329.51769160123007</v>
       </c>
       <c r="Y3">
         <v>0</v>
@@ -642,10 +642,10 @@
         <v>0</v>
       </c>
       <c r="AA3">
-        <v>2.3998557299008884E-2</v>
+        <v>9.5780000000000004E-2</v>
       </c>
       <c r="AB3">
-        <v>418.32270975413138</v>
+        <v>215.45084598552162</v>
       </c>
       <c r="AC3">
         <v>0</v>
@@ -659,10 +659,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>8012.0474625545867</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>418.2530912967265</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -671,10 +671,10 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>22.87088</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>339.25599792600491</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -683,49 +683,49 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>20915.296883265106</v>
+        <v>1648.5153813393476</v>
       </c>
       <c r="K4">
-        <v>18536.466660293354</v>
+        <v>489.00287567851819</v>
       </c>
       <c r="L4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>3.5543863002570238E-2</v>
+        <v>3.9824999999999999E-2</v>
       </c>
       <c r="N4">
-        <v>20802.088707995001</v>
+        <v>1514.6356721898792</v>
       </c>
       <c r="O4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>19244.538922948941</v>
+        <v>487.83340910654886</v>
       </c>
       <c r="R4">
-        <v>18536.466660293354</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>2.3055624770311308E-2</v>
+        <v>4.1812000000000002E-2</v>
       </c>
       <c r="U4">
-        <v>18921.309111453545</v>
+        <v>363.9943129835417</v>
       </c>
       <c r="V4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W4">
         <v>0</v>
       </c>
       <c r="X4">
-        <v>532.63102317939195</v>
+        <v>487.83340910654886</v>
       </c>
       <c r="Y4">
         <v>0</v>
@@ -734,10 +734,10 @@
         <v>0</v>
       </c>
       <c r="AA4">
-        <v>4.1771768799201733E-2</v>
+        <v>0.133516</v>
       </c>
       <c r="AB4">
-        <v>390.33571677624673</v>
+        <v>363.9943129835417</v>
       </c>
       <c r="AC4">
         <v>0</v>
@@ -751,10 +751,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>8794.4520636402158</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>522.36454437647365</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -763,10 +763,10 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>41.989404</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>423.56773141998332</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -775,49 +775,49 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>21408.914923198958</v>
+        <v>1829.479804082534</v>
       </c>
       <c r="K5">
-        <v>18937.125221963535</v>
+        <v>521.60306739041926</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>4.4440993188130259E-2</v>
+        <v>3.1487000000000001E-2</v>
       </c>
       <c r="N5">
-        <v>21156.25512321986</v>
+        <v>1620.6935200150481</v>
       </c>
       <c r="O5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>19853.217784146193</v>
+        <v>636.19764013783424</v>
       </c>
       <c r="R5">
-        <v>18937.125221963535</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <v>2.8037664963414786E-2</v>
+        <v>3.5194999999999997E-2</v>
       </c>
       <c r="U5">
-        <v>19280.140526678369</v>
+        <v>432.36396909680911</v>
       </c>
       <c r="V5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W5">
         <v>0</v>
       </c>
       <c r="X5">
-        <v>630.70438594655207</v>
+        <v>615.04052015403329</v>
       </c>
       <c r="Y5">
         <v>0</v>
@@ -826,10 +826,10 @@
         <v>0</v>
       </c>
       <c r="AA5">
-        <v>5.2773786077480324E-2</v>
+        <v>4.9773999999999999E-2</v>
       </c>
       <c r="AB5">
-        <v>466.14830888783263</v>
+        <v>438.11004647751957</v>
       </c>
       <c r="AC5">
         <v>0</v>
@@ -843,10 +843,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>9576.8566647258449</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>608.85563489670585</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -855,10 +855,10 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>212.25873200000001</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>482.48912759240784</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -867,49 +867,49 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>21945.177342471412</v>
+        <v>1943.3197688700625</v>
       </c>
       <c r="K6">
-        <v>19395.020721015175</v>
+        <v>558.86042934687839</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>4.3475020679093465E-2</v>
+        <v>7.7743999999999994E-2</v>
       </c>
       <c r="N6">
-        <v>21676.381264704567</v>
+        <v>1715.609157581878</v>
       </c>
       <c r="O6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>20437.49430504446</v>
+        <v>712.78024296890362</v>
       </c>
       <c r="R6">
-        <v>19395.020721015175</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>5.1096418619945003E-2</v>
+        <v>8.8526999999999995E-2</v>
       </c>
       <c r="U6">
-        <v>19794.551668163065</v>
+        <v>487.96424470718171</v>
       </c>
       <c r="V6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W6">
         <v>0</v>
       </c>
       <c r="X6">
-        <v>871.70748500309378</v>
+        <v>712.78024296890362</v>
       </c>
       <c r="Y6">
         <v>0</v>
@@ -918,10 +918,10 @@
         <v>0</v>
       </c>
       <c r="AA6">
-        <v>6.1822525022556425E-2</v>
+        <v>0.172623</v>
       </c>
       <c r="AB6">
-        <v>730.25254414923518</v>
+        <v>487.96424470718171</v>
       </c>
       <c r="AC6">
         <v>0</v>
@@ -935,10 +935,10 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>11481.430161610861</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>739.09684478648046</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -947,10 +947,10 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>546.54406700000004</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>587.85494115948563</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -959,49 +959,49 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>55328.337110708431</v>
+        <v>3037.8051981567664</v>
       </c>
       <c r="K7">
-        <v>52685.207835165646</v>
+        <v>1416.9754418424902</v>
       </c>
       <c r="L7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M7">
-        <v>3.6970350674189648E-2</v>
+        <v>4.3840999999999998E-2</v>
       </c>
       <c r="N7">
-        <v>55045.102794036102</v>
+        <v>2784.9378308375076</v>
       </c>
       <c r="O7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P7">
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>53833.42940173544</v>
+        <v>1512.1757754204339</v>
       </c>
       <c r="R7">
-        <v>52685.207835165653</v>
+        <v>708.487720921245</v>
       </c>
       <c r="S7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T7">
-        <v>3.9443308563932244E-2</v>
+        <v>4.7371999999999997E-2</v>
       </c>
       <c r="U7">
-        <v>53160.90119749459</v>
+        <v>1272.6421902764528</v>
       </c>
       <c r="V7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W7">
         <v>0</v>
       </c>
       <c r="X7">
-        <v>1014.1532551878734</v>
+        <v>1083.9061418862407</v>
       </c>
       <c r="Y7">
         <v>0</v>
@@ -1010,10 +1010,10 @@
         <v>0</v>
       </c>
       <c r="AA7">
-        <v>0.32835356869384358</v>
+        <v>0.268513</v>
       </c>
       <c r="AB7">
-        <v>782.9718564620332</v>
+        <v>891.93494327537439</v>
       </c>
       <c r="AC7">
         <v>0</v>
@@ -1027,10 +1027,10 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>12263.83476269649</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>878.09269802398217</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1039,10 +1039,10 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>7200.763927</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>695.52058371647865</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1051,49 +1051,49 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>60567.736133916282</v>
+        <v>3787.6455582478306</v>
       </c>
       <c r="K8">
-        <v>57781.636584276021</v>
+        <v>1535.0567286626965</v>
       </c>
       <c r="L8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M8">
-        <v>4.5575925552987971E-2</v>
+        <v>7.2527999999999995E-2</v>
       </c>
       <c r="N8">
-        <v>60226.4349094055</v>
+        <v>2987.6078306861555</v>
       </c>
       <c r="O8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>58994.062532449818</v>
+        <v>1848.7794416411598</v>
       </c>
       <c r="R8">
-        <v>57781.636584276021</v>
+        <v>767.52836433134826</v>
       </c>
       <c r="S8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T8">
-        <v>4.7037399861418784E-2</v>
+        <v>6.9191000000000003E-2</v>
       </c>
       <c r="U8">
-        <v>58345.031312864012</v>
+        <v>1420.4265467149955</v>
       </c>
       <c r="V8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="W8">
         <v>0</v>
       </c>
       <c r="X8">
-        <v>1095.7786130443003</v>
+        <v>1337.4892470773025</v>
       </c>
       <c r="Y8">
         <v>0</v>
@@ -1102,10 +1102,10 @@
         <v>0</v>
       </c>
       <c r="AA8">
-        <v>0.23251265492253448</v>
+        <v>0.18761700000000001</v>
       </c>
       <c r="AB8">
-        <v>814.33781538367464</v>
+        <v>895.80926917025306</v>
       </c>
       <c r="AC8">
         <v>0</v>
@@ -1119,10 +1119,10 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>13046.239363782119</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>982.18558581802893</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1131,10 +1131,10 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>7200.362537</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>797.20617468072646</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1143,49 +1143,49 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>62483.26710327663</v>
+        <v>4017.8846480789643</v>
       </c>
       <c r="K9">
-        <v>59618.170391417334</v>
+        <v>1674.6073403593068</v>
       </c>
       <c r="L9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M9">
-        <v>5.7682724110742094E-2</v>
+        <v>9.3383999999999995E-2</v>
       </c>
       <c r="N9">
-        <v>62118.431921620882</v>
+        <v>3191.2741581573682</v>
       </c>
       <c r="O9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>60943.880277231852</v>
+        <v>2009.2432256239883</v>
       </c>
       <c r="R9">
-        <v>59618.170391417334</v>
+        <v>837.30367017965341</v>
       </c>
       <c r="S9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T9">
-        <v>5.0879387694033613E-2</v>
+        <v>7.0768999999999999E-2</v>
       </c>
       <c r="U9">
-        <v>60240.592325079422</v>
+        <v>1549.7145683379042</v>
       </c>
       <c r="V9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="W9">
         <v>0</v>
       </c>
       <c r="X9">
-        <v>1227.4930050061523</v>
+        <v>1333.6265491332749</v>
       </c>
       <c r="Y9">
         <v>0</v>
@@ -1194,10 +1194,10 @@
         <v>0</v>
       </c>
       <c r="AA9">
-        <v>1.0649252423749043</v>
+        <v>0.30467</v>
       </c>
       <c r="AB9">
-        <v>874.93968417242274</v>
+        <v>1115.7736205568044</v>
       </c>
       <c r="AC9">
         <v>0</v>
@@ -1211,10 +1211,10 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>13828.643964867748</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1082.709759555491</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1223,10 +1223,10 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>7200.727817</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>812.20001168975</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1235,49 +1235,49 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>71594.86295082829</v>
+        <v>4967.7499832005233</v>
       </c>
       <c r="K10">
-        <v>66427.181145974944</v>
+        <v>1842.0680743952366</v>
       </c>
       <c r="L10">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M10">
-        <v>5.2305875365653023E-2</v>
+        <v>7.2266999999999998E-2</v>
       </c>
       <c r="N10">
-        <v>71227.895769172654</v>
+        <v>4139.4444932789247</v>
       </c>
       <c r="O10">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P10">
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>63263.301030696006</v>
+        <v>3123.3510947508516</v>
       </c>
       <c r="R10">
-        <v>61822.010959986859</v>
+        <v>1842.0680743952371</v>
       </c>
       <c r="S10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="T10">
-        <v>6.6884209592141142E-2</v>
+        <v>7.5253E-2</v>
       </c>
       <c r="U10">
-        <v>62547.437903997357</v>
+        <v>2630.9539421695445</v>
       </c>
       <c r="V10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="W10">
         <v>0</v>
       </c>
       <c r="X10">
-        <v>2826.1500983053807</v>
+        <v>1463.0684133476677</v>
       </c>
       <c r="Y10">
         <v>0</v>
@@ -1286,10 +1286,10 @@
         <v>0</v>
       </c>
       <c r="AA10">
-        <v>1.9646083146453492</v>
+        <v>0.99977700000000003</v>
       </c>
       <c r="AB10">
-        <v>1315.36879153985</v>
+        <v>1113.9669086852666</v>
       </c>
       <c r="AC10">
         <v>0</v>
@@ -1303,10 +1303,10 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>14749.678002065366</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1246.587578940751</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1315,10 +1315,10 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>7200.4716239999998</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>959.88206470852242</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1327,49 +1327,49 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>82219.572299392763</v>
+        <v>7116.8294033282982</v>
       </c>
       <c r="K11">
-        <v>74749.305401545382</v>
+        <v>3070.113457325393</v>
       </c>
       <c r="L11">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M11">
-        <v>5.4344202515169408E-2</v>
+        <v>7.7256000000000005E-2</v>
       </c>
       <c r="N11">
-        <v>81858.440117736987</v>
+        <v>6285.5969134066991</v>
       </c>
       <c r="O11">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="P11">
         <v>0</v>
       </c>
       <c r="Q11">
-        <v>66474.616538476053</v>
+        <v>4644.6436253947059</v>
       </c>
       <c r="R11">
-        <v>64515.593877127409</v>
+        <v>3070.113457325393</v>
       </c>
       <c r="S11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T11">
-        <v>6.3872514384343285E-2</v>
+        <v>9.0883000000000005E-2</v>
       </c>
       <c r="U11">
-        <v>65349.934634289442</v>
+        <v>3970.0228635298354</v>
       </c>
       <c r="V11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="W11">
         <v>0</v>
       </c>
       <c r="X11">
-        <v>1592.3628330484526</v>
+        <v>1810.1481978120398</v>
       </c>
       <c r="Y11">
         <v>0</v>
@@ -1378,10 +1378,10 @@
         <v>0</v>
       </c>
       <c r="AA11">
-        <v>7.4793399642965639</v>
+        <v>0.37156099999999997</v>
       </c>
       <c r="AB11">
-        <v>1345.2175270453586</v>
+        <v>1457.0850054802704</v>
       </c>
       <c r="AC11">
         <v>0</v>
@@ -1395,10 +1395,10 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>15670.712039262984</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1767.9251643847188</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1407,10 +1407,10 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>7200.2810749999999</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1086.509676997134</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1419,64 +1419,64 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>88821.7763890848</v>
+        <v>9914.5577553326839</v>
       </c>
       <c r="K12">
-        <v>79395.497988523333</v>
+        <v>5756.4627324851153</v>
       </c>
       <c r="L12">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M12">
-        <v>5.8377905739742657E-2</v>
+        <v>6.7581000000000002E-2</v>
       </c>
       <c r="N12">
-        <v>88445.919207429004</v>
+        <v>9036.3045843912023</v>
       </c>
       <c r="O12">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P12">
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>88735.309131999209</v>
+        <v>7645.5576570609828</v>
       </c>
       <c r="R12">
-        <v>86672.454876414064</v>
+        <v>5756.4627324851153</v>
       </c>
       <c r="S12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T12">
-        <v>6.9726376055714648E-2</v>
+        <v>7.4691999999999995E-2</v>
       </c>
       <c r="U12">
-        <v>87471.561876539388</v>
+        <v>6720.6665345143556</v>
       </c>
       <c r="V12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W12">
         <v>0</v>
       </c>
       <c r="X12">
-        <v>1870.3338046630006</v>
+        <v>5238.3037492820094</v>
       </c>
       <c r="Y12">
-        <v>0</v>
+        <v>3453.8776394910692</v>
       </c>
       <c r="Z12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA12">
-        <v>2.3509321805378725</v>
+        <v>4.0225299999999997</v>
       </c>
       <c r="AB12">
-        <v>1458.9098576314186</v>
+        <v>4717.6823336185471</v>
       </c>
       <c r="AC12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD12">
         <v>0</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1511,64 +1511,64 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>94919.778452457758</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <v>85369.174171780687</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="M13">
-        <v>6.6828458528604279E-2</v>
+        <v>0</v>
       </c>
       <c r="N13">
-        <v>94536.824523701041</v>
+        <v>0</v>
       </c>
       <c r="O13">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="P13">
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>94142.852696075628</v>
+        <v>0</v>
       </c>
       <c r="R13">
-        <v>91896.183724335715</v>
+        <v>0</v>
       </c>
       <c r="S13">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="T13">
-        <v>7.4912647185652173E-2</v>
+        <v>0</v>
       </c>
       <c r="U13">
-        <v>92808.291857475488</v>
+        <v>0</v>
       </c>
       <c r="V13">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="W13">
         <v>0</v>
       </c>
       <c r="X13">
-        <v>94142.852696075628</v>
+        <v>0</v>
       </c>
       <c r="Y13">
-        <v>91896.183724335715</v>
+        <v>0</v>
       </c>
       <c r="Z13">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AA13">
-        <v>9.3393843148364954</v>
+        <v>0</v>
       </c>
       <c r="AB13">
-        <v>92808.291857475488</v>
+        <v>0</v>
       </c>
       <c r="AC13">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AD13">
         <v>0</v>
@@ -1576,7 +1576,7 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1603,64 +1603,64 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>104840.6915328483</v>
+        <v>0</v>
       </c>
       <c r="K14">
-        <v>93334.075749457159</v>
+        <v>0</v>
       </c>
       <c r="L14">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="M14">
-        <v>6.8222235117026034E-2</v>
+        <v>0</v>
       </c>
       <c r="N14">
-        <v>104462.76260409155</v>
+        <v>0</v>
       </c>
       <c r="O14">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="P14">
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>101224.33909343324</v>
+        <v>0</v>
       </c>
       <c r="R14">
-        <v>98861.155521564564</v>
+        <v>0</v>
       </c>
       <c r="S14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="T14">
-        <v>9.8176769555823315E-2</v>
+        <v>0</v>
       </c>
       <c r="U14">
-        <v>99858.264475064701</v>
+        <v>0</v>
       </c>
       <c r="V14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="W14">
         <v>0</v>
       </c>
       <c r="X14">
-        <v>101224.33909343324</v>
+        <v>0</v>
       </c>
       <c r="Y14">
-        <v>98861.155521564564</v>
+        <v>0</v>
       </c>
       <c r="Z14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AA14">
-        <v>5.5232811890222742</v>
+        <v>0</v>
       </c>
       <c r="AB14">
-        <v>99858.264475064701</v>
+        <v>0</v>
       </c>
       <c r="AC14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AD14">
         <v>0</v>
@@ -1668,7 +1668,7 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1695,64 +1695,64 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>147839.69232343382</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>136243.1371536135</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="M15">
-        <v>7.4846371686651716E-2</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <v>147427.52406154003</v>
+        <v>0</v>
       </c>
       <c r="O15">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="P15">
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>142927.92483813508</v>
+        <v>0</v>
       </c>
       <c r="R15">
-        <v>140370.31523309427</v>
+        <v>0</v>
       </c>
       <c r="S15">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="T15">
-        <v>8.7120138990814722E-2</v>
+        <v>0</v>
       </c>
       <c r="U15">
-        <v>141431.0912398865</v>
+        <v>0</v>
       </c>
       <c r="V15">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="W15">
         <v>0</v>
       </c>
       <c r="X15">
-        <v>142927.92483813508</v>
+        <v>0</v>
       </c>
       <c r="Y15">
-        <v>140370.31523309427</v>
+        <v>0</v>
       </c>
       <c r="Z15">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AA15">
-        <v>3.3074847509463456</v>
+        <v>0</v>
       </c>
       <c r="AB15">
-        <v>141431.0912398865</v>
+        <v>0</v>
       </c>
       <c r="AC15">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AD15">
         <v>0</v>
@@ -1760,7 +1760,7 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1787,64 +1787,64 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>195258.01963256596</v>
+        <v>0</v>
       </c>
       <c r="K16">
-        <v>183498.59438313707</v>
+        <v>0</v>
       </c>
       <c r="L16">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="M16">
-        <v>7.6387774815765488E-2</v>
+        <v>0</v>
       </c>
       <c r="N16">
-        <v>194738.77103953919</v>
+        <v>0</v>
       </c>
       <c r="O16">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="P16">
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>187867.03657092812</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>185191.87757073811</v>
+        <v>0</v>
       </c>
       <c r="S16">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="T16">
-        <v>9.1602410721498412E-2</v>
+        <v>0</v>
       </c>
       <c r="U16">
-        <v>186309.6203260062</v>
+        <v>0</v>
       </c>
       <c r="V16">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="W16">
         <v>0</v>
       </c>
       <c r="X16">
-        <v>187867.03657092812</v>
+        <v>0</v>
       </c>
       <c r="Y16">
-        <v>185191.87757073811</v>
+        <v>0</v>
       </c>
       <c r="Z16">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AA16">
-        <v>1.5924986944011141</v>
+        <v>0</v>
       </c>
       <c r="AB16">
-        <v>186309.6203260062</v>
+        <v>0</v>
       </c>
       <c r="AC16">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AD16">
         <v>0</v>

</xml_diff>